<commit_message>
Improved the data workflow
</commit_message>
<xml_diff>
--- a/data/GTF BIG Talent Scholars.xlsx
+++ b/data/GTF BIG Talent Scholars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s2730428\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s2730428\Documents\GTF\global-talent-map\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B4C1D267-0B34-44E2-8E01-41AEEC38B3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D66817-5C70-4BAA-A515-B57ED673FF17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global Talent Fund - BIG Schola" sheetId="1" r:id="rId1"/>
@@ -360,7 +360,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -892,7 +892,11 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -903,6 +907,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27A1F45F-369C-43E2-9293-7A798EEDAE7D}" name="Table1" displayName="Table1" ref="A1:C78" totalsRowShown="0">
+  <autoFilter ref="A1:C78" xr:uid="{27A1F45F-369C-43E2-9293-7A798EEDAE7D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C78">
+    <sortCondition descending="1" ref="C1:C78"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{A1A6B3D3-D3CD-4920-BE0F-D040DB4E09C2}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{249ED221-263B-4AB2-86D0-DA07A7B1EB6A}" name="Country"/>
+    <tableColumn id="3" xr3:uid="{0133EB40-8B23-47E6-BCB0-B7D0E58418E9}" name="Year" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1201,11 +1220,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1228,370 +1247,370 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="C2" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C3" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="C4" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="C5" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C6" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C7" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C8" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="C9" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C10" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C11" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C12" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="C13" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="C14" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
         <v>84</v>
       </c>
       <c r="C15" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C16" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C17" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="C18" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C19" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C20" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="C21" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C22" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="C23" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C24" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="C25" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C26" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="C27" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C28" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="C29" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="C30" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C31" s="3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C32" s="3">
         <v>2025</v>
@@ -1600,10 +1619,10 @@
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C33" s="3">
         <v>2025</v>
@@ -1612,10 +1631,10 @@
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="B34" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="C34" s="3">
         <v>2025</v>
@@ -1624,10 +1643,10 @@
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="C35" s="3">
         <v>2025</v>
@@ -1636,10 +1655,10 @@
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="B36" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="C36" s="3">
         <v>2025</v>
@@ -1648,10 +1667,10 @@
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="B37" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C37" s="3">
         <v>2025</v>
@@ -1660,10 +1679,10 @@
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="B38" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="C38" s="3">
         <v>2025</v>
@@ -1672,10 +1691,10 @@
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="C39" s="3">
         <v>2025</v>
@@ -1684,10 +1703,10 @@
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="B40" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C40" s="3">
         <v>2025</v>
@@ -1696,10 +1715,10 @@
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="B41" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="C41" s="3">
         <v>2025</v>
@@ -1708,10 +1727,10 @@
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="B42" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="C42" s="3">
         <v>2025</v>
@@ -1720,10 +1739,10 @@
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="B43" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="C43" s="3">
         <v>2025</v>
@@ -1732,10 +1751,10 @@
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="B44" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C44" s="3">
         <v>2025</v>
@@ -1744,10 +1763,10 @@
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="B45" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C45" s="3">
         <v>2025</v>
@@ -1756,10 +1775,10 @@
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="B46" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C46" s="3">
         <v>2025</v>
@@ -1768,10 +1787,10 @@
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="B47" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C47" s="3">
         <v>2025</v>
@@ -1780,10 +1799,10 @@
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="B48" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C48" s="3">
         <v>2025</v>
@@ -1792,364 +1811,367 @@
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="B49" t="s">
         <v>80</v>
       </c>
       <c r="C49" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z49" s="1"/>
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C50" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z50" s="1"/>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="B51" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C51" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z51" s="1"/>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C52" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z52" s="1"/>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="C53" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z53" s="1"/>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="C54" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z54" s="1"/>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="B55" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="C55" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z55" s="1"/>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="B56" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C56" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z56" s="1"/>
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="C57" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z57" s="1"/>
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="B58" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C58" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z58" s="1"/>
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="B59" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C59" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z59" s="1"/>
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="B60" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C60" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z60" s="1"/>
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="B61" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C61" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="E61" s="2"/>
       <c r="Z61" s="1"/>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="B62" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="C62" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z62" s="1"/>
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
       <c r="B63" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C63" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z63" s="1"/>
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="B64" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="C64" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z64" s="1"/>
     </row>
     <row r="65" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>66</v>
+        <v>19</v>
       </c>
       <c r="B65" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C65" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z65" s="1"/>
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="B66" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C66" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z66" s="1"/>
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="B67" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C67" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z67" s="1"/>
     </row>
     <row r="68" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>69</v>
+        <v>22</v>
       </c>
       <c r="B68" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="C68" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z68" s="1"/>
     </row>
     <row r="69" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="B69" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="C69" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z69" s="1"/>
     </row>
     <row r="70" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="B70" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C70" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z70" s="1"/>
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="B71" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="C71" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z71" s="1"/>
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="B72" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="C72" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z72" s="1"/>
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="B73" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="C73" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z73" s="1"/>
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="B74" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="C74" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z74" s="1"/>
     </row>
     <row r="75" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="B75" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C75" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z75" s="1"/>
     </row>
     <row r="76" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>77</v>
+        <v>30</v>
       </c>
       <c r="B76" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C76" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="Z76" s="1"/>
     </row>
     <row r="77" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="B77" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C77" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="78" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>79</v>
+        <v>32</v>
       </c>
       <c r="B78" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C78" s="3">
-        <v>2025</v>
+        <v>2024</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>